<commit_message>
updated , user mode completed and business mode start
</commit_message>
<xml_diff>
--- a/Com.Synctag.com/ApplicationData/ApplicationTestData.xlsx
+++ b/Com.Synctag.com/ApplicationData/ApplicationTestData.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="11">
   <si>
     <t>Vinayak@56</t>
   </si>
@@ -25,15 +25,9 @@
     <t>amaravathi.hashinn@gmail.com</t>
   </si>
   <si>
-    <t>pragas.hashinn@gmail.com</t>
-  </si>
-  <si>
     <t>ranjithkumar.hashinn@gmail.com</t>
   </si>
   <si>
-    <t>prathapkumar.hashinn</t>
-  </si>
-  <si>
     <t>prathapkumar.hashinn@outlook.com</t>
   </si>
   <si>
@@ -50,6 +44,12 @@
   </si>
   <si>
     <t>Vimeo</t>
+  </si>
+  <si>
+    <t>prathapkumar.hashinn@gmail.com</t>
+  </si>
+  <si>
+    <t>Synctag@1</t>
   </si>
 </sst>
 </file>
@@ -96,9 +96,12 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -396,7 +399,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -407,7 +412,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -438,7 +443,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -446,7 +451,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -466,7 +471,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
@@ -475,8 +482,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
+      <c r="A1" s="2">
+        <v>7639416734</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -484,7 +491,7 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
@@ -492,15 +499,15 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>0</v>
@@ -508,10 +515,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1"/>
+    <hyperlink ref="A1" r:id="rId1" display="pragas.hashinn@gmail.com"/>
     <hyperlink ref="B1" r:id="rId2"/>
     <hyperlink ref="A2" r:id="rId3"/>
-    <hyperlink ref="A3" r:id="rId4" display="prathapkumar.hashinn@gmail.com"/>
+    <hyperlink ref="A3" r:id="rId4"/>
     <hyperlink ref="A4" r:id="rId5"/>
     <hyperlink ref="B2" r:id="rId6"/>
     <hyperlink ref="B3" r:id="rId7"/>
@@ -539,7 +546,7 @@
   <sheetData>
     <row r="1" spans="1:5">
       <c r="E1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -550,7 +557,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -561,18 +568,18 @@
         <v>0</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>